<commit_message>
Fixes rebase m.b.t. model reduction database
-Errors door niet-relative path db_carrides verholpen
</commit_message>
<xml_diff>
--- a/Output/export_kpis.xlsx
+++ b/Output/export_kpis.xlsx
@@ -268,7 +268,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>44715.48979581019</v>
+        <v>44715.54143104167</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
@@ -326,22 +326,22 @@
         <v>0.0</v>
       </c>
       <c r="T2" t="n">
-        <v>15.454241825954329</v>
+        <v>16.592177558161886</v>
       </c>
       <c r="U2" t="n">
-        <v>0.829404173501848</v>
+        <v>0.739408956016037</v>
       </c>
       <c r="V2" t="n">
-        <v>0.5238904142052863</v>
+        <v>0.6396518258887574</v>
       </c>
       <c r="W2" t="n">
-        <v>7400.0</v>
+        <v>6800.0</v>
       </c>
       <c r="X2" t="n">
-        <v>17.08</v>
+        <v>317.7</v>
       </c>
       <c r="Y2" t="n">
-        <v>58.26160002134016</v>
+        <v>55.15491297789812</v>
       </c>
       <c r="Z2" t="n">
         <v>0.0</v>
@@ -413,7 +413,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>44715.489796041664</v>
+        <v>44715.541431261576</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
@@ -471,22 +471,22 @@
         <v>0.0</v>
       </c>
       <c r="T3" t="n">
-        <v>16.98719153396851</v>
+        <v>17.36224718755243</v>
       </c>
       <c r="U3" t="n">
-        <v>1.016300061609272</v>
+        <v>1.2207691706471688</v>
       </c>
       <c r="V3" t="n">
-        <v>0.171536707002433</v>
+        <v>0.26595531990458554</v>
       </c>
       <c r="W3" t="n">
-        <v>9200.0</v>
+        <v>8200.0</v>
       </c>
       <c r="X3" t="n">
-        <v>18.96</v>
+        <v>296.77</v>
       </c>
       <c r="Y3" t="n">
-        <v>92.99548739041978</v>
+        <v>86.17726211857631</v>
       </c>
       <c r="Z3" t="n">
         <v>0.0</v>
@@ -558,7 +558,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>44715.48979612268</v>
+        <v>44715.54143131944</v>
       </c>
       <c r="C4" t="n">
         <v>2.0</v>
@@ -616,19 +616,19 @@
         <v>87.5</v>
       </c>
       <c r="T4" t="n">
-        <v>22.586786230566926</v>
+        <v>25.622597085337024</v>
       </c>
       <c r="U4" t="n">
-        <v>0.8249901178095191</v>
+        <v>1.818451052098019</v>
       </c>
       <c r="V4" t="n">
         <v>-0.0</v>
       </c>
       <c r="W4" t="n">
-        <v>5400.0</v>
+        <v>5800.0</v>
       </c>
       <c r="X4" t="n">
-        <v>9.73</v>
+        <v>198.71</v>
       </c>
       <c r="Y4" t="n">
         <v>100.0</v>
@@ -703,7 +703,7 @@
         <v>1.0</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>44715.48979620371</v>
+        <v>44715.54143143519</v>
       </c>
       <c r="C5" t="n">
         <v>3.0</v>
@@ -761,19 +761,19 @@
         <v>85.0</v>
       </c>
       <c r="T5" t="n">
-        <v>33.17347389292574</v>
+        <v>35.72940059895572</v>
       </c>
       <c r="U5" t="n">
-        <v>2.2012740486917943</v>
+        <v>3.272610974059578</v>
       </c>
       <c r="V5" t="n">
         <v>-0.0</v>
       </c>
       <c r="W5" t="n">
-        <v>6700.0</v>
+        <v>7200.0</v>
       </c>
       <c r="X5" t="n">
-        <v>7.11</v>
+        <v>111.04</v>
       </c>
       <c r="Y5" t="n">
         <v>100.0</v>
@@ -848,7 +848,7 @@
         <v>1.0</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>44715.48979623843</v>
+        <v>44715.54143145833</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1000,13 +1000,13 @@
         <v>69.0</v>
       </c>
       <c r="AH6" t="n">
-        <v>177.25784628770575</v>
+        <v>155.65267225175722</v>
       </c>
       <c r="AI6" t="n">
-        <v>64.37729369235434</v>
+        <v>47.16187409387012</v>
       </c>
       <c r="AJ6" t="n">
-        <v>58.94017944664275</v>
+        <v>58.15151520670435</v>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
@@ -1029,7 +1029,7 @@
         <v>1.0</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>44715.48979629629</v>
+        <v>44715.54143152778</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1207,10 +1207,960 @@
         </is>
       </c>
       <c r="AL7" t="n">
-        <v>2.6439206951031236</v>
+        <v>46.211079155152746</v>
       </c>
       <c r="AM7" t="n">
-        <v>3613.309218325836</v>
+        <v>47743.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>44715.54306967593</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>pop_buurten[0]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>rijtjeshuizen (laag)</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="L8" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P8" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>16.045884873030943</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.6845742062270038</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.6396518258887574</v>
+      </c>
+      <c r="W8" t="n">
+        <v>6600.0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>330.6</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>51.92390300909424</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>-2.5859575815597293</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>4.05959872840634</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>-5.858063759612174</v>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>44715.54306986111</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>pop_buurten[1]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>VVD-wijk (laag)</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="J9" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P9" t="n">
+        <v>92.5</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>14.14452876034304</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.6191124122990689</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.2739653785483065</v>
+      </c>
+      <c r="W9" t="n">
+        <v>7700.0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>341.2</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>77.4444014570355</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>-5.9241459786379025</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>14.969228292534202</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>-10.13360188854081</v>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>44715.54306991898</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>pop_buurten[2]</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>rijtjeshuizen (hoog)</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="L10" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="S10" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="T10" t="n">
+        <v>21.038341721770006</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.8699073342047108</v>
+      </c>
+      <c r="V10" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>5300.0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>270.74</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>-8.322974863051812</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>36.24300935079269</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>44715.543069976855</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>pop_buurten[3]</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>VVD-wijk (hoog)</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>77.5</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>72.5</v>
+      </c>
+      <c r="J11" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>24.82182455346574</v>
+      </c>
+      <c r="U11" t="n">
+        <v>1.5075240486917962</v>
+      </c>
+      <c r="V11" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>5900.0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>263.56</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>-17.423517264573913</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>137.35122953144509</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>44715.543070011576</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>holonAgent[0]</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>WindHolon</t>
+        </is>
+      </c>
+      <c r="AF12" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>137.83915743061382</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>30.55314281402029</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>51.20810434587503</v>
+      </c>
+      <c r="AK12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>44715.54307006944</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="AL13" t="n">
+        <v>60.30465406439814</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>40439.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes merge, carrides voor 40hh
-Fixes n.a.v. relative path carrides
-carrides voor 40 hh gegenereerd en ingevoerd
</commit_message>
<xml_diff>
--- a/Output/export_kpis.xlsx
+++ b/Output/export_kpis.xlsx
@@ -268,7 +268,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>44715.48979581019</v>
+        <v>44715.57863613426</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
@@ -326,22 +326,22 @@
         <v>0.0</v>
       </c>
       <c r="T2" t="n">
-        <v>15.454241825954329</v>
+        <v>16.3481348028805</v>
       </c>
       <c r="U2" t="n">
-        <v>0.829404173501848</v>
+        <v>0.8294041735018478</v>
       </c>
       <c r="V2" t="n">
-        <v>0.5238904142052863</v>
+        <v>0.6396518258887574</v>
       </c>
       <c r="W2" t="n">
-        <v>7400.0</v>
+        <v>6700.0</v>
       </c>
       <c r="X2" t="n">
-        <v>17.08</v>
+        <v>214.71</v>
       </c>
       <c r="Y2" t="n">
-        <v>58.26160002134016</v>
+        <v>53.91804380215612</v>
       </c>
       <c r="Z2" t="n">
         <v>0.0</v>
@@ -413,7 +413,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>44715.489796041664</v>
+        <v>44715.578636342594</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
@@ -471,22 +471,22 @@
         <v>0.0</v>
       </c>
       <c r="T3" t="n">
-        <v>16.98719153396851</v>
+        <v>15.653157735820223</v>
       </c>
       <c r="U3" t="n">
-        <v>1.016300061609272</v>
+        <v>1.150769170647169</v>
       </c>
       <c r="V3" t="n">
-        <v>0.171536707002433</v>
+        <v>0.2739653785483065</v>
       </c>
       <c r="W3" t="n">
-        <v>9200.0</v>
+        <v>7900.0</v>
       </c>
       <c r="X3" t="n">
-        <v>18.96</v>
+        <v>221.71</v>
       </c>
       <c r="Y3" t="n">
-        <v>92.99548739041978</v>
+        <v>81.8781765121124</v>
       </c>
       <c r="Z3" t="n">
         <v>0.0</v>
@@ -558,7 +558,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>44715.48979612268</v>
+        <v>44715.57863640046</v>
       </c>
       <c r="C4" t="n">
         <v>2.0</v>
@@ -616,19 +616,19 @@
         <v>87.5</v>
       </c>
       <c r="T4" t="n">
-        <v>22.586786230566926</v>
+        <v>23.39216620388452</v>
       </c>
       <c r="U4" t="n">
-        <v>0.8249901178095191</v>
+        <v>1.607201052098019</v>
       </c>
       <c r="V4" t="n">
         <v>-0.0</v>
       </c>
       <c r="W4" t="n">
-        <v>5400.0</v>
+        <v>5600.0</v>
       </c>
       <c r="X4" t="n">
-        <v>9.73</v>
+        <v>131.3</v>
       </c>
       <c r="Y4" t="n">
         <v>100.0</v>
@@ -703,7 +703,7 @@
         <v>1.0</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>44715.48979620371</v>
+        <v>44715.57863646991</v>
       </c>
       <c r="C5" t="n">
         <v>3.0</v>
@@ -761,19 +761,19 @@
         <v>85.0</v>
       </c>
       <c r="T5" t="n">
-        <v>33.17347389292574</v>
+        <v>30.032700517876982</v>
       </c>
       <c r="U5" t="n">
-        <v>2.2012740486917943</v>
+        <v>2.956545957017598</v>
       </c>
       <c r="V5" t="n">
         <v>-0.0</v>
       </c>
       <c r="W5" t="n">
-        <v>6700.0</v>
+        <v>6600.0</v>
       </c>
       <c r="X5" t="n">
-        <v>7.11</v>
+        <v>94.18</v>
       </c>
       <c r="Y5" t="n">
         <v>100.0</v>
@@ -848,7 +848,7 @@
         <v>1.0</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>44715.48979623843</v>
+        <v>44715.57863649305</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1000,13 +1000,13 @@
         <v>69.0</v>
       </c>
       <c r="AH6" t="n">
-        <v>177.25784628770575</v>
+        <v>147.13026571798542</v>
       </c>
       <c r="AI6" t="n">
-        <v>64.37729369235434</v>
+        <v>40.59442340173604</v>
       </c>
       <c r="AJ6" t="n">
-        <v>58.94017944664275</v>
+        <v>57.28768982389991</v>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
@@ -1029,7 +1029,7 @@
         <v>1.0</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>44715.48979629629</v>
+        <v>44715.578636516206</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1207,10 +1207,960 @@
         </is>
       </c>
       <c r="AL7" t="n">
-        <v>2.6439206951031236</v>
+        <v>33.0949220463136</v>
       </c>
       <c r="AM7" t="n">
-        <v>3613.309218325836</v>
+        <v>44032.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>44715.58029042824</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>pop_buurten[0]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>rijtjeshuizen (laag)</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>7.6923076923076925</v>
+      </c>
+      <c r="I8" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="L8" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P8" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>16.3481348028805</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.8294041735018478</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.6396518258887574</v>
+      </c>
+      <c r="W8" t="n">
+        <v>6700.0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>214.71</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>53.91804380215612</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.09904138006205263</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>-5.016326660606007E-4</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>44715.58029063657</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>pop_buurten[1]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>VVD-wijk (laag)</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="J9" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P9" t="n">
+        <v>92.5</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>15.653157735820223</v>
+      </c>
+      <c r="U9" t="n">
+        <v>1.150769170647169</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.2739653785483065</v>
+      </c>
+      <c r="W9" t="n">
+        <v>7900.0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>221.71</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>81.8781765121124</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0.39611086602817985</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>-0.0020463473673181807</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>44715.580290694445</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>pop_buurten[2]</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>rijtjeshuizen (hoog)</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>42.5531914893617</v>
+      </c>
+      <c r="I10" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="L10" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="S10" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="T10" t="n">
+        <v>23.39216620388452</v>
+      </c>
+      <c r="U10" t="n">
+        <v>1.607201052098019</v>
+      </c>
+      <c r="V10" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>5600.0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>131.3</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>-0.17531039169365872</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>-0.009039148214032521</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>44715.58029074074</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>pop_buurten[3]</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>VVD-wijk (hoog)</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>77.5</v>
+      </c>
+      <c r="H11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>72.5</v>
+      </c>
+      <c r="J11" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>30.032700517876982</v>
+      </c>
+      <c r="U11" t="n">
+        <v>2.956545957017598</v>
+      </c>
+      <c r="V11" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>6600.0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>94.18</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>-0.7120066804492732</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>-0.0027013259258631857</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>44715.580290763886</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>holonAgent[0]</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>WindHolon</t>
+        </is>
+      </c>
+      <c r="AF12" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>147.13026571798542</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>40.59442340173604</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>57.28768982389991</v>
+      </c>
+      <c r="AK12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>44715.58029078704</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="AL13" t="n">
+        <v>33.0949220463136</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>44032.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bijdrage districtheating aan HOLON energie consumptie
*efficiency van centrale warmtevoorziening en netwerk (afgeleverde warmte / primaire energie) gebruikt om primaire energiebehoefte warmtenet van HOLON-leden te berekenen.
</commit_message>
<xml_diff>
--- a/Output/export_kpis.xlsx
+++ b/Output/export_kpis.xlsx
@@ -65138,6 +65138,4056 @@
         <v>-99.0</v>
       </c>
     </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B289" s="3" t="n">
+        <v>44718.554736956015</v>
+      </c>
+      <c r="C289" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>pop_buurten[0]</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>B. Rijtjeswoningen</t>
+        </is>
+      </c>
+      <c r="F289" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G289" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H289" t="n">
+        <v>58.333333333333336</v>
+      </c>
+      <c r="I289" t="n">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="J289" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K289" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L289" t="n">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="M289" t="n">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="N289" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O289" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P289" t="n">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="Q289" t="n">
+        <v>86.66666666666667</v>
+      </c>
+      <c r="R289" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S289" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T289" t="n">
+        <v>31.51058143010344</v>
+      </c>
+      <c r="U289" t="n">
+        <v>2.2790254442345246</v>
+      </c>
+      <c r="V289" t="n">
+        <v>0.30811867476361215</v>
+      </c>
+      <c r="W289" t="n">
+        <v>4600.0</v>
+      </c>
+      <c r="X289" t="n">
+        <v>100.36</v>
+      </c>
+      <c r="Y289" t="n">
+        <v>89.52505606516209</v>
+      </c>
+      <c r="Z289" t="n">
+        <v>0.3812610803039285</v>
+      </c>
+      <c r="AA289" t="n">
+        <v>-0.0033176074022353056</v>
+      </c>
+      <c r="AB289" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC289" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="AD289" t="n">
+        <v>7442.0</v>
+      </c>
+      <c r="AE289" t="n">
+        <v>319.0</v>
+      </c>
+      <c r="AF289" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="AG289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB289" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B290" s="3" t="n">
+        <v>44718.554737060185</v>
+      </c>
+      <c r="C290" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>pop_buurten[1]</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>C. Villawijk</t>
+        </is>
+      </c>
+      <c r="F290" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G290" t="n">
+        <v>86.66666666666667</v>
+      </c>
+      <c r="H290" t="n">
+        <v>31.25</v>
+      </c>
+      <c r="I290" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="J290" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K290" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L290" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M290" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N290" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O290" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P290" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q290" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="R290" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S290" t="n">
+        <v>93.33333333333333</v>
+      </c>
+      <c r="T290" t="n">
+        <v>26.133646092028112</v>
+      </c>
+      <c r="U290" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V290" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="W290" t="n">
+        <v>5000.0</v>
+      </c>
+      <c r="X290" t="n">
+        <v>93.59</v>
+      </c>
+      <c r="Y290" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="Z290" t="n">
+        <v>0.023502001271626796</v>
+      </c>
+      <c r="AA290" t="n">
+        <v>-0.007082598081379105</v>
+      </c>
+      <c r="AB290" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC290" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="AD290" t="n">
+        <v>23128.0</v>
+      </c>
+      <c r="AE290" t="n">
+        <v>356.0</v>
+      </c>
+      <c r="AF290" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="AG290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB290" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B291" s="3" t="n">
+        <v>44718.55473707176</v>
+      </c>
+      <c r="C291" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>pop_buurten[2]</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>D. Rijtjeswoningen</t>
+        </is>
+      </c>
+      <c r="F291" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G291" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="H291" t="n">
+        <v>16.216216216216218</v>
+      </c>
+      <c r="I291" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J291" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K291" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L291" t="n">
+        <v>73.33333333333333</v>
+      </c>
+      <c r="M291" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="N291" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O291" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P291" t="n">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="Q291" t="n">
+        <v>76.66666666666667</v>
+      </c>
+      <c r="R291" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S291" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T291" t="n">
+        <v>33.28879656414257</v>
+      </c>
+      <c r="U291" t="n">
+        <v>1.429669847391185</v>
+      </c>
+      <c r="V291" t="n">
+        <v>1.4080182048259688</v>
+      </c>
+      <c r="W291" t="n">
+        <v>3700.0</v>
+      </c>
+      <c r="X291" t="n">
+        <v>103.57</v>
+      </c>
+      <c r="Y291" t="n">
+        <v>44.534772363203224</v>
+      </c>
+      <c r="Z291" t="n">
+        <v>0.3405000476924903</v>
+      </c>
+      <c r="AA291" t="n">
+        <v>-0.015667995459482307</v>
+      </c>
+      <c r="AB291" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC291" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="AD291" t="n">
+        <v>6628.0</v>
+      </c>
+      <c r="AE291" t="n">
+        <v>459.0</v>
+      </c>
+      <c r="AF291" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="AG291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB291" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B292" s="3" t="n">
+        <v>44718.554737094906</v>
+      </c>
+      <c r="C292" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>pop_buurten[3]</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>A. Villawijk</t>
+        </is>
+      </c>
+      <c r="F292" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G292" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="H292" t="n">
+        <v>38.46153846153846</v>
+      </c>
+      <c r="I292" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="J292" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O292" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P292" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="Q292" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="R292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T292" t="n">
+        <v>25.881289317286715</v>
+      </c>
+      <c r="U292" t="n">
+        <v>1.568577424483491</v>
+      </c>
+      <c r="V292" t="n">
+        <v>1.1707929012809182</v>
+      </c>
+      <c r="W292" t="n">
+        <v>5400.0</v>
+      </c>
+      <c r="X292" t="n">
+        <v>132.13</v>
+      </c>
+      <c r="Y292" t="n">
+        <v>51.38090396391826</v>
+      </c>
+      <c r="Z292" t="n">
+        <v>-0.09813596746666749</v>
+      </c>
+      <c r="AA292" t="n">
+        <v>0.0011189229310391018</v>
+      </c>
+      <c r="AB292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC292" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="AD292" t="n">
+        <v>6138.0</v>
+      </c>
+      <c r="AE292" t="n">
+        <v>640.0</v>
+      </c>
+      <c r="AF292" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="AG292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB292" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="B293" s="3" t="n">
+        <v>44718.55473710648</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG293" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH293" t="inlineStr">
+        <is>
+          <t>holonAgent[0]</t>
+        </is>
+      </c>
+      <c r="AI293" t="inlineStr">
+        <is>
+          <t>WindHolon</t>
+        </is>
+      </c>
+      <c r="AJ293" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL293" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM293" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="AN293" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="AO293" t="n">
+        <v>124.36667782542435</v>
+      </c>
+      <c r="AP293" t="n">
+        <v>28.74333868811022</v>
+      </c>
+      <c r="AQ293" t="n">
+        <v>25.285148759350704</v>
+      </c>
+      <c r="AR293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS293" t="n">
+        <v>97098.0</v>
+      </c>
+      <c r="AT293" t="n">
+        <v>397.0</v>
+      </c>
+      <c r="AU293" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="AV293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB293" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B294" s="3" t="n">
+        <v>44718.55473711806</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU294" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV294" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="AW294" t="n">
+        <v>28.642806306700273</v>
+      </c>
+      <c r="AX294" t="n">
+        <v>48062.0</v>
+      </c>
+      <c r="AY294" t="n">
+        <v>99.15953196347031</v>
+      </c>
+      <c r="AZ294" t="n">
+        <v>10834.09526986352</v>
+      </c>
+      <c r="BA294" t="n">
+        <v>118.33881566831127</v>
+      </c>
+      <c r="BB294" t="n">
+        <v>-99.0</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B295" s="3" t="n">
+        <v>44718.55720002315</v>
+      </c>
+      <c r="C295" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>pop_buurten[0]</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>B. Rijtjeswoningen</t>
+        </is>
+      </c>
+      <c r="F295" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G295" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H295" t="n">
+        <v>58.333333333333336</v>
+      </c>
+      <c r="I295" t="n">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="J295" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K295" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L295" t="n">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="M295" t="n">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="N295" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O295" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P295" t="n">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="Q295" t="n">
+        <v>86.66666666666667</v>
+      </c>
+      <c r="R295" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S295" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T295" t="n">
+        <v>31.51058143010344</v>
+      </c>
+      <c r="U295" t="n">
+        <v>2.2790254442345246</v>
+      </c>
+      <c r="V295" t="n">
+        <v>0.30811867476361215</v>
+      </c>
+      <c r="W295" t="n">
+        <v>4600.0</v>
+      </c>
+      <c r="X295" t="n">
+        <v>100.36</v>
+      </c>
+      <c r="Y295" t="n">
+        <v>89.52505606516209</v>
+      </c>
+      <c r="Z295" t="n">
+        <v>0.3812610803039285</v>
+      </c>
+      <c r="AA295" t="n">
+        <v>-0.0033176074022353056</v>
+      </c>
+      <c r="AB295" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC295" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="AD295" t="n">
+        <v>7442.0</v>
+      </c>
+      <c r="AE295" t="n">
+        <v>319.0</v>
+      </c>
+      <c r="AF295" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="AG295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB295" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B296" s="3" t="n">
+        <v>44718.557200104166</v>
+      </c>
+      <c r="C296" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>pop_buurten[1]</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>C. Villawijk</t>
+        </is>
+      </c>
+      <c r="F296" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G296" t="n">
+        <v>86.66666666666667</v>
+      </c>
+      <c r="H296" t="n">
+        <v>31.25</v>
+      </c>
+      <c r="I296" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="J296" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O296" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q296" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="R296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S296" t="n">
+        <v>93.33333333333333</v>
+      </c>
+      <c r="T296" t="n">
+        <v>26.133646092028112</v>
+      </c>
+      <c r="U296" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V296" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="W296" t="n">
+        <v>5000.0</v>
+      </c>
+      <c r="X296" t="n">
+        <v>93.59</v>
+      </c>
+      <c r="Y296" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="Z296" t="n">
+        <v>0.023502001271626796</v>
+      </c>
+      <c r="AA296" t="n">
+        <v>-0.007082598081379105</v>
+      </c>
+      <c r="AB296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC296" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="AD296" t="n">
+        <v>23128.0</v>
+      </c>
+      <c r="AE296" t="n">
+        <v>356.0</v>
+      </c>
+      <c r="AF296" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="AG296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB296" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B297" s="3" t="n">
+        <v>44718.55720012732</v>
+      </c>
+      <c r="C297" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>pop_buurten[2]</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>D. Rijtjeswoningen</t>
+        </is>
+      </c>
+      <c r="F297" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G297" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="H297" t="n">
+        <v>16.216216216216218</v>
+      </c>
+      <c r="I297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K297" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L297" t="n">
+        <v>73.33333333333333</v>
+      </c>
+      <c r="M297" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="N297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O297" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P297" t="n">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="Q297" t="n">
+        <v>76.66666666666667</v>
+      </c>
+      <c r="R297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T297" t="n">
+        <v>33.28879656414257</v>
+      </c>
+      <c r="U297" t="n">
+        <v>1.429669847391185</v>
+      </c>
+      <c r="V297" t="n">
+        <v>1.4080182048259688</v>
+      </c>
+      <c r="W297" t="n">
+        <v>3700.0</v>
+      </c>
+      <c r="X297" t="n">
+        <v>103.57</v>
+      </c>
+      <c r="Y297" t="n">
+        <v>44.534772363203224</v>
+      </c>
+      <c r="Z297" t="n">
+        <v>0.3405000476924903</v>
+      </c>
+      <c r="AA297" t="n">
+        <v>-0.015667995459482307</v>
+      </c>
+      <c r="AB297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC297" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="AD297" t="n">
+        <v>6628.0</v>
+      </c>
+      <c r="AE297" t="n">
+        <v>459.0</v>
+      </c>
+      <c r="AF297" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="AG297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB297" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B298" s="3" t="n">
+        <v>44718.55720015046</v>
+      </c>
+      <c r="C298" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>pop_buurten[3]</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>A. Villawijk</t>
+        </is>
+      </c>
+      <c r="F298" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G298" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="H298" t="n">
+        <v>38.46153846153846</v>
+      </c>
+      <c r="I298" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="J298" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O298" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P298" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="Q298" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="R298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T298" t="n">
+        <v>25.881289317286715</v>
+      </c>
+      <c r="U298" t="n">
+        <v>1.568577424483491</v>
+      </c>
+      <c r="V298" t="n">
+        <v>1.1707929012809182</v>
+      </c>
+      <c r="W298" t="n">
+        <v>5400.0</v>
+      </c>
+      <c r="X298" t="n">
+        <v>132.13</v>
+      </c>
+      <c r="Y298" t="n">
+        <v>51.38090396391826</v>
+      </c>
+      <c r="Z298" t="n">
+        <v>-0.09813596746666749</v>
+      </c>
+      <c r="AA298" t="n">
+        <v>0.0011189229310391018</v>
+      </c>
+      <c r="AB298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC298" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="AD298" t="n">
+        <v>6138.0</v>
+      </c>
+      <c r="AE298" t="n">
+        <v>640.0</v>
+      </c>
+      <c r="AF298" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="AG298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB298" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B299" s="3" t="n">
+        <v>44718.55720016204</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG299" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH299" t="inlineStr">
+        <is>
+          <t>holonAgent[0]</t>
+        </is>
+      </c>
+      <c r="AI299" t="inlineStr">
+        <is>
+          <t>WindHolon</t>
+        </is>
+      </c>
+      <c r="AJ299" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL299" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM299" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="AN299" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="AO299" t="n">
+        <v>124.36667782542435</v>
+      </c>
+      <c r="AP299" t="n">
+        <v>28.74333868811022</v>
+      </c>
+      <c r="AQ299" t="n">
+        <v>25.285148759350704</v>
+      </c>
+      <c r="AR299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS299" t="n">
+        <v>97098.0</v>
+      </c>
+      <c r="AT299" t="n">
+        <v>397.0</v>
+      </c>
+      <c r="AU299" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="AV299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB299" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B300" s="3" t="n">
+        <v>44718.55720016204</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU300" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV300" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="AW300" t="n">
+        <v>28.642806306700273</v>
+      </c>
+      <c r="AX300" t="n">
+        <v>48062.0</v>
+      </c>
+      <c r="AY300" t="n">
+        <v>99.15953196347031</v>
+      </c>
+      <c r="AZ300" t="n">
+        <v>10834.09526986352</v>
+      </c>
+      <c r="BA300" t="n">
+        <v>118.33881566831127</v>
+      </c>
+      <c r="BB300" t="n">
+        <v>-99.0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="B301" s="3" t="n">
+        <v>44718.57063165509</v>
+      </c>
+      <c r="C301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>pop_buurten[0]</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>B. Rijtjeswoningen</t>
+        </is>
+      </c>
+      <c r="F301" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G301" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H301" t="n">
+        <v>58.333333333333336</v>
+      </c>
+      <c r="I301" t="n">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="J301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K301" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L301" t="n">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="M301" t="n">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="N301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O301" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P301" t="n">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="Q301" t="n">
+        <v>86.66666666666667</v>
+      </c>
+      <c r="R301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T301" t="n">
+        <v>31.51058143010344</v>
+      </c>
+      <c r="U301" t="n">
+        <v>2.2790254442345246</v>
+      </c>
+      <c r="V301" t="n">
+        <v>0.30811867476361215</v>
+      </c>
+      <c r="W301" t="n">
+        <v>4600.0</v>
+      </c>
+      <c r="X301" t="n">
+        <v>100.36</v>
+      </c>
+      <c r="Y301" t="n">
+        <v>89.52505606516209</v>
+      </c>
+      <c r="Z301" t="n">
+        <v>0.3812610803039285</v>
+      </c>
+      <c r="AA301" t="n">
+        <v>-0.0033176074022353056</v>
+      </c>
+      <c r="AB301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC301" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="AD301" t="n">
+        <v>7442.0</v>
+      </c>
+      <c r="AE301" t="n">
+        <v>319.0</v>
+      </c>
+      <c r="AF301" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="AG301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB301" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="B302" s="3" t="n">
+        <v>44718.57063174769</v>
+      </c>
+      <c r="C302" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>pop_buurten[1]</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>C. Villawijk</t>
+        </is>
+      </c>
+      <c r="F302" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G302" t="n">
+        <v>86.66666666666667</v>
+      </c>
+      <c r="H302" t="n">
+        <v>31.25</v>
+      </c>
+      <c r="I302" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="J302" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O302" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q302" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="R302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S302" t="n">
+        <v>93.33333333333333</v>
+      </c>
+      <c r="T302" t="n">
+        <v>26.133646092028112</v>
+      </c>
+      <c r="U302" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V302" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="W302" t="n">
+        <v>5000.0</v>
+      </c>
+      <c r="X302" t="n">
+        <v>93.59</v>
+      </c>
+      <c r="Y302" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="Z302" t="n">
+        <v>0.023502001271626796</v>
+      </c>
+      <c r="AA302" t="n">
+        <v>-0.007082598081379105</v>
+      </c>
+      <c r="AB302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC302" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="AD302" t="n">
+        <v>23128.0</v>
+      </c>
+      <c r="AE302" t="n">
+        <v>356.0</v>
+      </c>
+      <c r="AF302" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="AG302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB302" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="B303" s="3" t="n">
+        <v>44718.57063177083</v>
+      </c>
+      <c r="C303" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>pop_buurten[2]</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>D. Rijtjeswoningen</t>
+        </is>
+      </c>
+      <c r="F303" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G303" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="H303" t="n">
+        <v>16.216216216216218</v>
+      </c>
+      <c r="I303" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J303" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K303" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L303" t="n">
+        <v>73.33333333333333</v>
+      </c>
+      <c r="M303" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="N303" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O303" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P303" t="n">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="Q303" t="n">
+        <v>76.66666666666667</v>
+      </c>
+      <c r="R303" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S303" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T303" t="n">
+        <v>33.28879656414257</v>
+      </c>
+      <c r="U303" t="n">
+        <v>1.429669847391185</v>
+      </c>
+      <c r="V303" t="n">
+        <v>1.4080182048259688</v>
+      </c>
+      <c r="W303" t="n">
+        <v>3700.0</v>
+      </c>
+      <c r="X303" t="n">
+        <v>103.57</v>
+      </c>
+      <c r="Y303" t="n">
+        <v>44.534772363203224</v>
+      </c>
+      <c r="Z303" t="n">
+        <v>0.3405000476924903</v>
+      </c>
+      <c r="AA303" t="n">
+        <v>-0.015667995459482307</v>
+      </c>
+      <c r="AB303" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC303" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="AD303" t="n">
+        <v>6628.0</v>
+      </c>
+      <c r="AE303" t="n">
+        <v>459.0</v>
+      </c>
+      <c r="AF303" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="AG303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB303" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="B304" s="3" t="n">
+        <v>44718.570631793984</v>
+      </c>
+      <c r="C304" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>pop_buurten[3]</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>A. Villawijk</t>
+        </is>
+      </c>
+      <c r="F304" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G304" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="H304" t="n">
+        <v>38.46153846153846</v>
+      </c>
+      <c r="I304" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="J304" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O304" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P304" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="Q304" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="R304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T304" t="n">
+        <v>25.881289317286715</v>
+      </c>
+      <c r="U304" t="n">
+        <v>1.568577424483491</v>
+      </c>
+      <c r="V304" t="n">
+        <v>1.1707929012809182</v>
+      </c>
+      <c r="W304" t="n">
+        <v>5400.0</v>
+      </c>
+      <c r="X304" t="n">
+        <v>132.13</v>
+      </c>
+      <c r="Y304" t="n">
+        <v>51.38090396391826</v>
+      </c>
+      <c r="Z304" t="n">
+        <v>-0.09813596746666749</v>
+      </c>
+      <c r="AA304" t="n">
+        <v>0.0011189229310391018</v>
+      </c>
+      <c r="AB304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC304" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="AD304" t="n">
+        <v>6138.0</v>
+      </c>
+      <c r="AE304" t="n">
+        <v>640.0</v>
+      </c>
+      <c r="AF304" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="AG304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB304" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B305" s="3" t="n">
+        <v>44718.57063180555</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG305" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH305" t="inlineStr">
+        <is>
+          <t>holonAgent[0]</t>
+        </is>
+      </c>
+      <c r="AI305" t="inlineStr">
+        <is>
+          <t>WindHolon</t>
+        </is>
+      </c>
+      <c r="AJ305" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL305" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM305" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="AN305" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="AO305" t="n">
+        <v>124.36667782542435</v>
+      </c>
+      <c r="AP305" t="n">
+        <v>28.74333868811022</v>
+      </c>
+      <c r="AQ305" t="n">
+        <v>25.234815727644598</v>
+      </c>
+      <c r="AR305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS305" t="n">
+        <v>97098.0</v>
+      </c>
+      <c r="AT305" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="AU305" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="AV305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB305" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="B306" s="3" t="n">
+        <v>44718.57063181713</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU306" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV306" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="AW306" t="n">
+        <v>28.642806306700273</v>
+      </c>
+      <c r="AX306" t="n">
+        <v>48062.0</v>
+      </c>
+      <c r="AY306" t="n">
+        <v>99.15953196347031</v>
+      </c>
+      <c r="AZ306" t="n">
+        <v>10834.09526986352</v>
+      </c>
+      <c r="BA306" t="n">
+        <v>118.33881566831127</v>
+      </c>
+      <c r="BB306" t="n">
+        <v>-99.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
District heating opwek+buffer en netwerk als populaties in main gezet, zodat huishoudens in alle wijken aangesloten kunnen worden
Let op! Berekening van KPIs, en ook de energiebalans van de district heating werkt nu wel alleen correct als er slechts in 1 buurt aansluitingen zijn. Als er in meer buurten aansluitingen zijn, wordt de energiebalans van de district-heating meerdere keren per tijdstap aangeroepen. Dat moet nog gefixt worden!
</commit_message>
<xml_diff>
--- a/Output/export_kpis.xlsx
+++ b/Output/export_kpis.xlsx
@@ -86738,6 +86738,2706 @@
         <v>-99.0</v>
       </c>
     </row>
+    <row r="385">
+      <c r="A385" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B385" s="3" t="n">
+        <v>44728.74669502315</v>
+      </c>
+      <c r="C385" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>pop_buurten[0]</t>
+        </is>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>B. Rijtjeswoningen</t>
+        </is>
+      </c>
+      <c r="F385" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G385" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H385" t="n">
+        <v>58.333333333333336</v>
+      </c>
+      <c r="I385" t="n">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="J385" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K385" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L385" t="n">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="M385" t="n">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="N385" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O385" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P385" t="n">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="Q385" t="n">
+        <v>86.66666666666667</v>
+      </c>
+      <c r="R385" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S385" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T385" t="n">
+        <v>25.46618636191116</v>
+      </c>
+      <c r="U385" t="n">
+        <v>1.630778385743953</v>
+      </c>
+      <c r="V385" t="n">
+        <v>0.30811867476361215</v>
+      </c>
+      <c r="W385" t="n">
+        <v>4000.0</v>
+      </c>
+      <c r="X385" t="n">
+        <v>11.12</v>
+      </c>
+      <c r="Y385" t="n">
+        <v>84.89940391898718</v>
+      </c>
+      <c r="Z385" t="n">
+        <v>-10.16162475353285</v>
+      </c>
+      <c r="AA385" t="n">
+        <v>-86.02073003295988</v>
+      </c>
+      <c r="AB385" t="n">
+        <v>0.42389937566875835</v>
+      </c>
+      <c r="AC385" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="AD385" t="n">
+        <v>6169.0</v>
+      </c>
+      <c r="AE385" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="AF385" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="AG385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB385" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B386" s="3" t="n">
+        <v>44728.746695104164</v>
+      </c>
+      <c r="C386" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>pop_buurten[1]</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>C. Villawijk</t>
+        </is>
+      </c>
+      <c r="F386" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G386" t="n">
+        <v>86.66666666666667</v>
+      </c>
+      <c r="H386" t="n">
+        <v>31.25</v>
+      </c>
+      <c r="I386" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="J386" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K386" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L386" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M386" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N386" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O386" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P386" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q386" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="R386" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S386" t="n">
+        <v>93.33333333333333</v>
+      </c>
+      <c r="T386" t="n">
+        <v>8.11186907354841</v>
+      </c>
+      <c r="U386" t="n">
+        <v>0.5979000917821877</v>
+      </c>
+      <c r="V386" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="W386" t="n">
+        <v>3200.0</v>
+      </c>
+      <c r="X386" t="n">
+        <v>6.93</v>
+      </c>
+      <c r="Y386" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="Z386" t="n">
+        <v>-35.13666419135154</v>
+      </c>
+      <c r="AA386" t="n">
+        <v>-91.65945726896652</v>
+      </c>
+      <c r="AB386" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC386" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="AD386" t="n">
+        <v>22478.0</v>
+      </c>
+      <c r="AE386" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="AF386" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="AG386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB386" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B387" s="3" t="n">
+        <v>44728.746695127316</v>
+      </c>
+      <c r="C387" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>pop_buurten[2]</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>D. Rijtjeswoningen</t>
+        </is>
+      </c>
+      <c r="F387" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G387" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="H387" t="n">
+        <v>16.216216216216218</v>
+      </c>
+      <c r="I387" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J387" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K387" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L387" t="n">
+        <v>73.33333333333333</v>
+      </c>
+      <c r="M387" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="N387" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O387" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P387" t="n">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="Q387" t="n">
+        <v>76.66666666666667</v>
+      </c>
+      <c r="R387" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S387" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T387" t="n">
+        <v>34.740714184150015</v>
+      </c>
+      <c r="U387" t="n">
+        <v>1.292292948236146</v>
+      </c>
+      <c r="V387" t="n">
+        <v>1.4137189456117336</v>
+      </c>
+      <c r="W387" t="n">
+        <v>2800.0</v>
+      </c>
+      <c r="X387" t="n">
+        <v>4.64</v>
+      </c>
+      <c r="Y387" t="n">
+        <v>39.77498804251507</v>
+      </c>
+      <c r="Z387" t="n">
+        <v>-24.11979903525545</v>
+      </c>
+      <c r="AA387" t="n">
+        <v>-92.37423794261464</v>
+      </c>
+      <c r="AB387" t="n">
+        <v>-4.987789293136892</v>
+      </c>
+      <c r="AC387" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="AD387" t="n">
+        <v>5729.0</v>
+      </c>
+      <c r="AE387" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="AF387" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="AG387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB387" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B388" s="3" t="n">
+        <v>44728.74669515046</v>
+      </c>
+      <c r="C388" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>pop_buurten[3]</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>A. Villawijk</t>
+        </is>
+      </c>
+      <c r="F388" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G388" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="H388" t="n">
+        <v>38.46153846153846</v>
+      </c>
+      <c r="I388" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="J388" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K388" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L388" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M388" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N388" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O388" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P388" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="Q388" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="R388" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S388" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T388" t="n">
+        <v>27.410131567729007</v>
+      </c>
+      <c r="U388" t="n">
+        <v>0.8446924907150006</v>
+      </c>
+      <c r="V388" t="n">
+        <v>1.1856447013973996</v>
+      </c>
+      <c r="W388" t="n">
+        <v>4600.0</v>
+      </c>
+      <c r="X388" t="n">
+        <v>12.22</v>
+      </c>
+      <c r="Y388" t="n">
+        <v>43.41766378957561</v>
+      </c>
+      <c r="Z388" t="n">
+        <v>-15.54991205088301</v>
+      </c>
+      <c r="AA388" t="n">
+        <v>-88.19579490755613</v>
+      </c>
+      <c r="AB388" t="n">
+        <v>-5.143728636720557</v>
+      </c>
+      <c r="AC388" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="AD388" t="n">
+        <v>4474.0</v>
+      </c>
+      <c r="AE388" t="n">
+        <v>88.0</v>
+      </c>
+      <c r="AF388" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="AG388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB388" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="B389" s="3" t="n">
+        <v>44728.74669515046</v>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG389" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH389" t="inlineStr">
+        <is>
+          <t>holonAgent[0]</t>
+        </is>
+      </c>
+      <c r="AI389" t="inlineStr">
+        <is>
+          <t>WindHolon</t>
+        </is>
+      </c>
+      <c r="AJ389" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL389" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM389" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="AN389" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="AO389" t="n">
+        <v>113.98225451271271</v>
+      </c>
+      <c r="AP389" t="n">
+        <v>36.31528637725874</v>
+      </c>
+      <c r="AQ389" t="n">
+        <v>25.37548555583892</v>
+      </c>
+      <c r="AR389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS389" t="n">
+        <v>16008.0</v>
+      </c>
+      <c r="AT389" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="AU389" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="AV389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB389" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B390" s="3" t="n">
+        <v>44728.74669519676</v>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU390" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV390" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="AW390" t="n">
+        <v>2.326872547442524</v>
+      </c>
+      <c r="AX390" t="n">
+        <v>7052.0</v>
+      </c>
+      <c r="AY390" t="n">
+        <v>99.75</v>
+      </c>
+      <c r="AZ390" t="n">
+        <v>9712.539616648808</v>
+      </c>
+      <c r="BA390" t="n">
+        <v>14.971353006192516</v>
+      </c>
+      <c r="BB390" t="n">
+        <v>-99.0</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="B391" s="3" t="n">
+        <v>44728.75161148148</v>
+      </c>
+      <c r="C391" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>pop_buurten[0]</t>
+        </is>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>B. Rijtjeswoningen</t>
+        </is>
+      </c>
+      <c r="F391" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G391" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H391" t="n">
+        <v>58.333333333333336</v>
+      </c>
+      <c r="I391" t="n">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="J391" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K391" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L391" t="n">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="M391" t="n">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="N391" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O391" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P391" t="n">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="Q391" t="n">
+        <v>86.66666666666667</v>
+      </c>
+      <c r="R391" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S391" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T391" t="n">
+        <v>30.51570715030555</v>
+      </c>
+      <c r="U391" t="n">
+        <v>1.6563013558301172</v>
+      </c>
+      <c r="V391" t="n">
+        <v>0.32385804060187795</v>
+      </c>
+      <c r="W391" t="n">
+        <v>4500.0</v>
+      </c>
+      <c r="X391" t="n">
+        <v>79.52</v>
+      </c>
+      <c r="Y391" t="n">
+        <v>84.54103499944064</v>
+      </c>
+      <c r="Z391" t="n">
+        <v>12.701213253023298</v>
+      </c>
+      <c r="AA391" t="n">
+        <v>615.130522188807</v>
+      </c>
+      <c r="AB391" t="n">
+        <v>-0.42211005378612393</v>
+      </c>
+      <c r="AC391" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="AD391" t="n">
+        <v>7259.0</v>
+      </c>
+      <c r="AE391" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="AF391" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="AG391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB391" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="B392" s="3" t="n">
+        <v>44728.75161157407</v>
+      </c>
+      <c r="C392" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>pop_buurten[1]</t>
+        </is>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>C. Villawijk</t>
+        </is>
+      </c>
+      <c r="F392" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G392" t="n">
+        <v>86.66666666666667</v>
+      </c>
+      <c r="H392" t="n">
+        <v>31.25</v>
+      </c>
+      <c r="I392" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="J392" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K392" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L392" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M392" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N392" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O392" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P392" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q392" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="R392" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S392" t="n">
+        <v>93.33333333333333</v>
+      </c>
+      <c r="T392" t="n">
+        <v>26.782843037304342</v>
+      </c>
+      <c r="U392" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V392" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="W392" t="n">
+        <v>4800.0</v>
+      </c>
+      <c r="X392" t="n">
+        <v>81.38</v>
+      </c>
+      <c r="Y392" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="Z392" t="n">
+        <v>51.45811826972482</v>
+      </c>
+      <c r="AA392" t="n">
+        <v>1074.3525280837025</v>
+      </c>
+      <c r="AB392" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC392" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="AD392" t="n">
+        <v>23394.0</v>
+      </c>
+      <c r="AE392" t="n">
+        <v>305.0</v>
+      </c>
+      <c r="AF392" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="AG392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB392" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="B393" s="3" t="n">
+        <v>44728.751611597225</v>
+      </c>
+      <c r="C393" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>pop_buurten[2]</t>
+        </is>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>D. Rijtjeswoningen</t>
+        </is>
+      </c>
+      <c r="F393" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G393" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="H393" t="n">
+        <v>16.216216216216218</v>
+      </c>
+      <c r="I393" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J393" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K393" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L393" t="n">
+        <v>73.33333333333333</v>
+      </c>
+      <c r="M393" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="N393" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O393" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P393" t="n">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="Q393" t="n">
+        <v>76.66666666666667</v>
+      </c>
+      <c r="R393" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S393" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T393" t="n">
+        <v>33.495949185477755</v>
+      </c>
+      <c r="U393" t="n">
+        <v>1.429669847391185</v>
+      </c>
+      <c r="V393" t="n">
+        <v>1.4137189456117336</v>
+      </c>
+      <c r="W393" t="n">
+        <v>3700.0</v>
+      </c>
+      <c r="X393" t="n">
+        <v>60.92</v>
+      </c>
+      <c r="Y393" t="n">
+        <v>41.86302765360449</v>
+      </c>
+      <c r="Z393" t="n">
+        <v>30.798801573853535</v>
+      </c>
+      <c r="AA393" t="n">
+        <v>1212.9224481675892</v>
+      </c>
+      <c r="AB393" t="n">
+        <v>5.249629764457848</v>
+      </c>
+      <c r="AC393" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="AD393" t="n">
+        <v>6608.0</v>
+      </c>
+      <c r="AE393" t="n">
+        <v>325.0</v>
+      </c>
+      <c r="AF393" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="AG393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB393" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="B394" s="3" t="n">
+        <v>44728.751611631946</v>
+      </c>
+      <c r="C394" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>pop_buurten[3]</t>
+        </is>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>A. Villawijk</t>
+        </is>
+      </c>
+      <c r="F394" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G394" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="H394" t="n">
+        <v>38.46153846153846</v>
+      </c>
+      <c r="I394" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="J394" t="n">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K394" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L394" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M394" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N394" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O394" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P394" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="Q394" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="R394" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S394" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T394" t="n">
+        <v>26.83631878503719</v>
+      </c>
+      <c r="U394" t="n">
+        <v>1.1170052414094649</v>
+      </c>
+      <c r="V394" t="n">
+        <v>1.1856447013973996</v>
+      </c>
+      <c r="W394" t="n">
+        <v>5400.0</v>
+      </c>
+      <c r="X394" t="n">
+        <v>103.55</v>
+      </c>
+      <c r="Y394" t="n">
+        <v>45.77205404089219</v>
+      </c>
+      <c r="Z394" t="n">
+        <v>16.65870217831112</v>
+      </c>
+      <c r="AA394" t="n">
+        <v>747.3889543749675</v>
+      </c>
+      <c r="AB394" t="n">
+        <v>5.42265531081352</v>
+      </c>
+      <c r="AC394" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="AD394" t="n">
+        <v>6026.0</v>
+      </c>
+      <c r="AE394" t="n">
+        <v>551.0</v>
+      </c>
+      <c r="AF394" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="AG394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB394" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B395" s="3" t="n">
+        <v>44728.75161164352</v>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG395" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH395" t="inlineStr">
+        <is>
+          <t>holonAgent[0]</t>
+        </is>
+      </c>
+      <c r="AI395" t="inlineStr">
+        <is>
+          <t>WindHolon</t>
+        </is>
+      </c>
+      <c r="AJ395" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL395" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM395" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="AN395" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="AO395" t="n">
+        <v>122.52460981160796</v>
+      </c>
+      <c r="AP395" t="n">
+        <v>27.149351480758565</v>
+      </c>
+      <c r="AQ395" t="n">
+        <v>29.512149165536368</v>
+      </c>
+      <c r="AR395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS395" t="n">
+        <v>96159.0</v>
+      </c>
+      <c r="AT395" t="n">
+        <v>321.0</v>
+      </c>
+      <c r="AU395" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="AV395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BB395" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="B396" s="3" t="n">
+        <v>44728.75161167824</v>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="U396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AJ396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AK396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AU396" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV396" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="AW396" t="n">
+        <v>21.692021197924706</v>
+      </c>
+      <c r="AX396" t="n">
+        <v>47022.0</v>
+      </c>
+      <c r="AY396" t="n">
+        <v>99.18093607305936</v>
+      </c>
+      <c r="AZ396" t="n">
+        <v>10821.672537630362</v>
+      </c>
+      <c r="BA396" t="n">
+        <v>95.80089748258845</v>
+      </c>
+      <c r="BB396" t="n">
+        <v>-99.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>